<commit_message>
Introdotti dati plausibili. ¡¡¡Attenzione al separatore decimale!!!
</commit_message>
<xml_diff>
--- a/debug-excel/Load_Profiles 060107 073113.xlsx
+++ b/debug-excel/Load_Profiles 060107 073113.xlsx
@@ -55,7 +55,7 @@
     <numFmt formatCode="0.0" numFmtId="166"/>
     <numFmt formatCode="GENERAL" numFmtId="167"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -77,6 +77,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +152,3054 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$4:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$4:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>21.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.07</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28.84</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.77</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.69</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.11</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$H$4:$H$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>21.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.59</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.07</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.89</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.66</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.52</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25.79</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.76</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.528</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.74</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.86</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.62</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.76</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$4:$J$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>19.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.08</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.07</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28.84</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.77</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.707E-008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.343E-008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.947E-009</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.674E-007</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.148E-008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="0"/>
+        <c:axId val="94083490"/>
+        <c:axId val="91167840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="94083490"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="91167840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="91167840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+          <c:min val="-10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="94083490"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$U$4:$U$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>50.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>112.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>126.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>158.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>137.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>127.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>123.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>139.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>143.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>131.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>115.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>98.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>87.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>73.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>52.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$V$4:$V$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>50.300045433122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.1235908301523</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.0441465579103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.2535210669565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.503670741494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.7240893206687</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.3466759514418</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105.826114279163</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>112.582486592983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>126.255733277851</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>158.768864299332</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149.024096539015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>137.139301348982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125.223934338523</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>127.547392690787</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>123.068620998595</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>139.065326035727</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>143.826887066846</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>131.559944121506</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>115.188734284174</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>98.7563808059921</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>87.8728127348616</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>73.7180598783072</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>52.2795708056099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$W$4:$W$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.002447</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.002127</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.005064</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00173</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.004733</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.003006</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.003909</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.003339</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.002974</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>479.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>487.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>495.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>455.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>466</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$X$4:$X$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="0"/>
+        <c:axId val="31715518"/>
+        <c:axId val="45471147"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="31715518"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="45471147"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45471147"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="31715518"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>734760</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>159480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>176400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3028320" y="5223600"/>
+        <a:ext cx="7851600" cy="5616720"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>309240</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>720720</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>101880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="11777040" y="6111720"/>
+        <a:ext cx="5763240" cy="3245040"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -157,8 +3209,8 @@
   </sheetPr>
   <dimension ref="C2:AK27"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="O18" activeCellId="0" pane="topLeft" sqref="O18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="E9" activeCellId="0" pane="topLeft" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.75"/>
@@ -223,34 +3275,34 @@
         <v>25</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>431.2</v>
+        <v>250.3</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>25</v>
+        <v>21.69</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>-0.09378</v>
+        <v>-1.563E-005</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>25</v>
+        <v>21.01</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>-97.89</v>
+        <v>-50.3</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>-333.2</v>
+        <v>19.01</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>431.2</v>
+        <v>250.3</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>-97.89</v>
+        <v>-50.3</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>-333.2</v>
+        <v>-200</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="0" t="n">
@@ -260,10 +3312,27 @@
         <v>25</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>97.9444696850678</v>
+        <v>50.300045433122</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="3" t="n">
+        <f aca="false">-I4</f>
+        <v>50.3</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <f aca="false">R4</f>
+        <v>50.300045433122</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <f aca="false">-K4</f>
+        <v>200</v>
+      </c>
+      <c r="X4" s="3" t="n">
+        <f aca="false">S4</f>
+        <v>200</v>
       </c>
       <c r="AD4" s="0" t="n">
         <v>147.258514464293</v>
@@ -298,34 +3367,34 @@
         <v>25</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>423.9</v>
+        <v>237.1</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>25</v>
+        <v>21.99</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.1848</v>
+        <v>-0.0001923</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>25</v>
+        <v>21.59</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>-90.81</v>
+        <v>-37.1</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>-333.2</v>
+        <v>19.31</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>423.9</v>
+        <v>237.1</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>-90.81</v>
+        <v>-37.1</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>-333.2</v>
+        <v>-200</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="0" t="n">
@@ -335,10 +3404,27 @@
         <v>25</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>90.6242171278624</v>
+        <v>37.1235908301523</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="3" t="n">
+        <f aca="false">-I5</f>
+        <v>37.1</v>
+      </c>
+      <c r="V5" s="3" t="n">
+        <f aca="false">R5</f>
+        <v>37.1235908301523</v>
+      </c>
+      <c r="W5" s="3" t="n">
+        <f aca="false">-K5</f>
+        <v>200</v>
+      </c>
+      <c r="X5" s="3" t="n">
+        <f aca="false">S5</f>
+        <v>200</v>
       </c>
       <c r="AD5" s="0" t="n">
         <v>0</v>
@@ -373,34 +3459,34 @@
         <v>25</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>429.4</v>
+        <v>247</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>25</v>
+        <v>21.76</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0.1972</v>
+        <v>-3.044E-005</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>25</v>
+        <v>21.16</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>-96.46</v>
+        <v>-47</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>-333.1</v>
+        <v>19.09</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>429.4</v>
+        <v>247</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>-96.46</v>
+        <v>-47</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>-333.1</v>
+        <v>-200</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="0" t="n">
@@ -410,10 +3496,27 @@
         <v>25</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>96.1356369766168</v>
+        <v>47.0441465579103</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="3" t="n">
+        <f aca="false">-I6</f>
+        <v>47</v>
+      </c>
+      <c r="V6" s="3" t="n">
+        <f aca="false">R6</f>
+        <v>47.0441465579103</v>
+      </c>
+      <c r="W6" s="3" t="n">
+        <f aca="false">-K6</f>
+        <v>200</v>
+      </c>
+      <c r="X6" s="3" t="n">
+        <f aca="false">S6</f>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="7">
@@ -424,34 +3527,34 @@
         <v>25</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>423.9</v>
+        <v>237.3</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>25</v>
+        <v>21.99</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>0.369</v>
+        <v>5.864E-005</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>25</v>
+        <v>21.59</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>-90.95</v>
+        <v>-37.3</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>-333.3</v>
+        <v>19.31</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>423.9</v>
+        <v>237.3</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>-90.95</v>
+        <v>-37.3</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>-333.3</v>
+        <v>-200</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="0" t="n">
@@ -461,10 +3564,27 @@
         <v>25</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>90.6964005927536</v>
+        <v>37.2535210669565</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="3" t="n">
+        <f aca="false">-I7</f>
+        <v>37.3</v>
+      </c>
+      <c r="V7" s="3" t="n">
+        <f aca="false">R7</f>
+        <v>37.2535210669565</v>
+      </c>
+      <c r="W7" s="3" t="n">
+        <f aca="false">-K7</f>
+        <v>200</v>
+      </c>
+      <c r="X7" s="3" t="n">
+        <f aca="false">S7</f>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="8">
@@ -475,34 +3595,34 @@
         <v>25</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>433.6</v>
+        <v>254.5</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>25</v>
+        <v>21.59</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-0.1347</v>
+        <v>-0.0001988</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>25</v>
+        <v>20.81</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>-100.1</v>
+        <v>-54.5</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>-333.4</v>
+        <v>18.91</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>433.6</v>
+        <v>254.5</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>-100.1</v>
+        <v>-54.5</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>-333.4</v>
+        <v>-200</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="0" t="n">
@@ -512,10 +3632,27 @@
         <v>25</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>100.279817078608</v>
+        <v>54.503670741494</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="3" t="n">
+        <f aca="false">-I8</f>
+        <v>54.5</v>
+      </c>
+      <c r="V8" s="3" t="n">
+        <f aca="false">R8</f>
+        <v>54.503670741494</v>
+      </c>
+      <c r="W8" s="3" t="n">
+        <f aca="false">-K8</f>
+        <v>200</v>
+      </c>
+      <c r="X8" s="3" t="n">
+        <f aca="false">S8</f>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="9">
@@ -526,34 +3663,34 @@
         <v>25</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>433.1</v>
+        <v>253.7</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>25</v>
+        <v>21.61</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0.2063</v>
+        <v>1.912E-005</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>25</v>
+        <v>20.85</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>-100.1</v>
+        <v>-53.7</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>-333.2</v>
+        <v>18.93</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>433.1</v>
+        <v>253.7</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>-100.1</v>
+        <v>-53.7</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>-333.2</v>
+        <v>-200</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="0" t="n">
@@ -563,10 +3700,27 @@
         <v>25</v>
       </c>
       <c r="R9" s="2" t="n">
-        <v>99.8467162892604</v>
+        <v>53.7240893206687</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="3" t="n">
+        <f aca="false">-I9</f>
+        <v>53.7</v>
+      </c>
+      <c r="V9" s="3" t="n">
+        <f aca="false">R9</f>
+        <v>53.7240893206687</v>
+      </c>
+      <c r="W9" s="3" t="n">
+        <f aca="false">-K9</f>
+        <v>200</v>
+      </c>
+      <c r="X9" s="3" t="n">
+        <f aca="false">S9</f>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="10">
@@ -577,34 +3731,34 @@
         <v>30</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>452.4</v>
+        <v>288.3</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>30</v>
+        <v>25.75</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>-0.2247</v>
+        <v>2.475E-005</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>30</v>
+        <v>23.93</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>-119.1</v>
+        <v>-88.3</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>-333.1</v>
+        <v>23.08</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>452.4</v>
+        <v>288.3</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>-119.1</v>
+        <v>-88.3</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>-333.1</v>
+        <v>-200</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="0" t="n">
@@ -614,10 +3768,27 @@
         <v>30</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>119.08148663969</v>
+        <v>88.3466759514418</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="3" t="n">
+        <f aca="false">-I10</f>
+        <v>88.3</v>
+      </c>
+      <c r="V10" s="3" t="n">
+        <f aca="false">R10</f>
+        <v>88.3466759514418</v>
+      </c>
+      <c r="W10" s="3" t="n">
+        <f aca="false">-K10</f>
+        <v>200</v>
+      </c>
+      <c r="X10" s="3" t="n">
+        <f aca="false">S10</f>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="11">
@@ -628,34 +3799,34 @@
         <v>30</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>462.1</v>
+        <v>305.8</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>30</v>
+        <v>25.27</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>-0.1629</v>
+        <v>-4.146E-005</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>30</v>
+        <v>22.76</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>-128.6</v>
+        <v>-105.8</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>-333.3</v>
+        <v>22.6</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>462.1</v>
+        <v>305.8</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>-128.6</v>
+        <v>-105.8</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>-333.3</v>
+        <v>-200</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="0" t="n">
@@ -665,10 +3836,27 @@
         <v>30</v>
       </c>
       <c r="R11" s="2" t="n">
-        <v>128.792285710646</v>
+        <v>105.826114279163</v>
       </c>
       <c r="S11" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="3" t="n">
+        <f aca="false">-I11</f>
+        <v>105.8</v>
+      </c>
+      <c r="V11" s="3" t="n">
+        <f aca="false">R11</f>
+        <v>105.826114279163</v>
+      </c>
+      <c r="W11" s="3" t="n">
+        <f aca="false">-K11</f>
+        <v>200</v>
+      </c>
+      <c r="X11" s="3" t="n">
+        <f aca="false">S11</f>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="12">
@@ -679,34 +3867,34 @@
         <v>30</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>465.6</v>
+        <v>312.6</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>30</v>
+        <v>25.08</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.1102</v>
+        <v>-0.0001373</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>30</v>
+        <v>22.28</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>-132.6</v>
+        <v>-112.6</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>-333.2</v>
+        <v>22.41</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>-200</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>465.6</v>
+        <v>312.6</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>-132.6</v>
+        <v>-112.6</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>-333.2</v>
+        <v>-200</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="0" t="n">
@@ -716,10 +3904,27 @@
         <v>30</v>
       </c>
       <c r="R12" s="2" t="n">
-        <v>132.545825884991</v>
+        <v>112.582486592983</v>
       </c>
       <c r="S12" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>200</v>
+      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="3" t="n">
+        <f aca="false">-I12</f>
+        <v>112.6</v>
+      </c>
+      <c r="V12" s="3" t="n">
+        <f aca="false">R12</f>
+        <v>112.582486592983</v>
+      </c>
+      <c r="W12" s="3" t="n">
+        <f aca="false">-K12</f>
+        <v>200</v>
+      </c>
+      <c r="X12" s="3" t="n">
+        <f aca="false">S12</f>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="13">
@@ -730,34 +3935,34 @@
         <v>30</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>142.2</v>
+        <v>126.3</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>30</v>
+        <v>29.02</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>33.69</v>
+        <v>-0.002447</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>30</v>
+        <v>25.59</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>-140</v>
+        <v>-126.3</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>-35.89</v>
+        <v>29.02</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>0.002447</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>142.2</v>
+        <v>126.3</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>-140</v>
+        <v>-126.3</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>-35.89</v>
+        <v>0.002447</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="0" t="n">
@@ -767,9 +3972,26 @@
         <v>30</v>
       </c>
       <c r="R13" s="2" t="n">
-        <v>140.142074043251</v>
+        <v>126.255733277851</v>
       </c>
       <c r="S13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="3" t="n">
+        <f aca="false">-I13</f>
+        <v>126.3</v>
+      </c>
+      <c r="V13" s="3" t="n">
+        <f aca="false">R13</f>
+        <v>126.255733277851</v>
+      </c>
+      <c r="W13" s="3" t="n">
+        <f aca="false">-K13</f>
+        <v>-0.002447</v>
+      </c>
+      <c r="X13" s="3" t="n">
+        <f aca="false">S13</f>
         <v>0</v>
       </c>
     </row>
@@ -781,34 +4003,34 @@
         <v>30</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>158.7</v>
+        <v>158.8</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>30</v>
+        <v>28.54</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>-40.06</v>
+        <v>0.002127</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>30</v>
+        <v>23.35</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>-158.1</v>
+        <v>-158.8</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>39.46</v>
+        <v>28.54</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>-0.002127</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>158.7</v>
+        <v>158.8</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>-158.1</v>
+        <v>-158.8</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>39.46</v>
+        <v>-0.002127</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="0" t="n">
@@ -818,9 +4040,26 @@
         <v>30</v>
       </c>
       <c r="R14" s="2" t="n">
-        <v>158.20492461074</v>
+        <v>158.768864299332</v>
       </c>
       <c r="S14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" s="3" t="n">
+        <f aca="false">-I14</f>
+        <v>158.8</v>
+      </c>
+      <c r="V14" s="3" t="n">
+        <f aca="false">R14</f>
+        <v>158.768864299332</v>
+      </c>
+      <c r="W14" s="3" t="n">
+        <f aca="false">-K14</f>
+        <v>0.002127</v>
+      </c>
+      <c r="X14" s="3" t="n">
+        <f aca="false">S14</f>
         <v>0</v>
       </c>
     </row>
@@ -832,34 +4071,34 @@
         <v>30</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>152.9</v>
+        <v>149</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>30</v>
+        <v>28.69</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>21.67</v>
+        <v>-0.005082</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>30</v>
+        <v>24.07</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>-152.7</v>
+        <v>-149</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>-21.91</v>
+        <v>28.69</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>0.005064</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>152.9</v>
+        <v>149</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>-152.7</v>
+        <v>-149</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>-21.91</v>
+        <v>0.005064</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" s="0" t="n">
@@ -869,9 +4108,26 @@
         <v>30</v>
       </c>
       <c r="R15" s="2" t="n">
-        <v>152.791164743897</v>
+        <v>149.024096539015</v>
       </c>
       <c r="S15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="3" t="n">
+        <f aca="false">-I15</f>
+        <v>149</v>
+      </c>
+      <c r="V15" s="3" t="n">
+        <f aca="false">R15</f>
+        <v>149.024096539015</v>
+      </c>
+      <c r="W15" s="3" t="n">
+        <f aca="false">-K15</f>
+        <v>-0.005064</v>
+      </c>
+      <c r="X15" s="3" t="n">
+        <f aca="false">S15</f>
         <v>0</v>
       </c>
     </row>
@@ -883,34 +4139,34 @@
         <v>30</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>146.4</v>
+        <v>137.1</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>30</v>
+        <v>28.87</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>-47.65</v>
+        <v>0.00173</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>30</v>
+        <v>24.89</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>-146</v>
+        <v>-137.1</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>47.33</v>
+        <v>28.87</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>-0.00173</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>146.4</v>
+        <v>137.1</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>-146</v>
+        <v>-137.1</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>47.33</v>
+        <v>-0.00173</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="0" t="n">
@@ -920,9 +4176,26 @@
         <v>30</v>
       </c>
       <c r="R16" s="2" t="n">
-        <v>146.188500749434</v>
+        <v>137.139301348982</v>
       </c>
       <c r="S16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="3" t="n">
+        <f aca="false">-I16</f>
+        <v>137.1</v>
+      </c>
+      <c r="V16" s="3" t="n">
+        <f aca="false">R16</f>
+        <v>137.139301348982</v>
+      </c>
+      <c r="W16" s="3" t="n">
+        <f aca="false">-K16</f>
+        <v>0.00173</v>
+      </c>
+      <c r="X16" s="3" t="n">
+        <f aca="false">S16</f>
         <v>0</v>
       </c>
     </row>
@@ -934,34 +4207,34 @@
         <v>30</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>141.2</v>
+        <v>125.2</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>30</v>
+        <v>29.04</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>33.88</v>
+        <v>-0.004733</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>30</v>
+        <v>25.66</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>-139.4</v>
+        <v>-125.2</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>-35.66</v>
+        <v>29.04</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>0.004733</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>141.2</v>
+        <v>125.2</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>-139.4</v>
+        <v>-125.2</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>-35.66</v>
+        <v>0.004733</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="0" t="n">
@@ -971,9 +4244,26 @@
         <v>30</v>
       </c>
       <c r="R17" s="2" t="n">
-        <v>139.568852410291</v>
+        <v>125.223934338523</v>
       </c>
       <c r="S17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="3" t="n">
+        <f aca="false">-I17</f>
+        <v>125.2</v>
+      </c>
+      <c r="V17" s="3" t="n">
+        <f aca="false">R17</f>
+        <v>125.223934338523</v>
+      </c>
+      <c r="W17" s="3" t="n">
+        <f aca="false">-K17</f>
+        <v>-0.004733</v>
+      </c>
+      <c r="X17" s="3" t="n">
+        <f aca="false">S17</f>
         <v>0</v>
       </c>
     </row>
@@ -985,34 +4275,34 @@
         <v>30</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>141.3</v>
+        <v>127.5</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>30</v>
+        <v>29.01</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>-40.1</v>
+        <v>0.003006</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>30</v>
+        <v>25.52</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>-140.8</v>
+        <v>-127.5</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>39.66</v>
+        <v>29.01</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>-0.003006</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>141.3</v>
+        <v>127.5</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>-140.8</v>
+        <v>-127.5</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>39.66</v>
+        <v>-0.003006</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="0" t="n">
@@ -1022,9 +4312,26 @@
         <v>30</v>
       </c>
       <c r="R18" s="2" t="n">
-        <v>140.859662605993</v>
+        <v>127.547392690787</v>
       </c>
       <c r="S18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2"/>
+      <c r="U18" s="3" t="n">
+        <f aca="false">-I18</f>
+        <v>127.5</v>
+      </c>
+      <c r="V18" s="3" t="n">
+        <f aca="false">R18</f>
+        <v>127.547392690787</v>
+      </c>
+      <c r="W18" s="3" t="n">
+        <f aca="false">-K18</f>
+        <v>0.003006</v>
+      </c>
+      <c r="X18" s="3" t="n">
+        <f aca="false">S18</f>
         <v>0</v>
       </c>
     </row>
@@ -1036,34 +4343,34 @@
         <v>30</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>139.7</v>
+        <v>123.1</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>30</v>
+        <v>29.07</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>-25.03</v>
+        <v>-0.003909</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>30</v>
+        <v>25.79</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>-138.3</v>
+        <v>-123.1</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <v>23.67</v>
+        <v>29.07</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>0.003909</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>139.7</v>
+        <v>123.1</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>-138.3</v>
+        <v>-123.1</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>23.67</v>
+        <v>0.003909</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="0" t="n">
@@ -1073,9 +4380,26 @@
         <v>30</v>
       </c>
       <c r="R19" s="2" t="n">
-        <v>138.37145611033</v>
+        <v>123.068620998595</v>
       </c>
       <c r="S19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="3" t="n">
+        <f aca="false">-I19</f>
+        <v>123.1</v>
+      </c>
+      <c r="V19" s="3" t="n">
+        <f aca="false">R19</f>
+        <v>123.068620998595</v>
+      </c>
+      <c r="W19" s="3" t="n">
+        <f aca="false">-K19</f>
+        <v>-0.003909</v>
+      </c>
+      <c r="X19" s="3" t="n">
+        <f aca="false">S19</f>
         <v>0</v>
       </c>
     </row>
@@ -1087,34 +4411,34 @@
         <v>30</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>147.3</v>
+        <v>139.1</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>30</v>
+        <v>28.84</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>-47.58</v>
+        <v>0.003339</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>30</v>
+        <v>24.76</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>-147.2</v>
+        <v>-139.1</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <v>47.48</v>
+        <v>28.84</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>-0.003339</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>147.3</v>
+        <v>139.1</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>-147.2</v>
+        <v>-139.1</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>47.48</v>
+        <v>-0.003339</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="0" t="n">
@@ -1124,9 +4448,26 @@
         <v>30</v>
       </c>
       <c r="R20" s="2" t="n">
-        <v>147.258514464293</v>
+        <v>139.065326035727</v>
       </c>
       <c r="S20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="3" t="n">
+        <f aca="false">-I20</f>
+        <v>139.1</v>
+      </c>
+      <c r="V20" s="3" t="n">
+        <f aca="false">R20</f>
+        <v>139.065326035727</v>
+      </c>
+      <c r="W20" s="3" t="n">
+        <f aca="false">-K20</f>
+        <v>0.003339</v>
+      </c>
+      <c r="X20" s="3" t="n">
+        <f aca="false">S20</f>
         <v>0</v>
       </c>
     </row>
@@ -1138,34 +4479,34 @@
         <v>30</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>149.9</v>
+        <v>143.8</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>30</v>
+        <v>28.77</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>21.21</v>
+        <v>0.002974</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>30</v>
+        <v>24.44</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>-149.8</v>
+        <v>-143.8</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <v>-21.21</v>
+        <v>28.77</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>-0.002974</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>149.9</v>
+        <v>143.8</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>-149.8</v>
+        <v>-143.8</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>-21.21</v>
+        <v>-0.002974</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="0" t="n">
@@ -1175,9 +4516,26 @@
         <v>30</v>
       </c>
       <c r="R21" s="2" t="n">
-        <v>149.903826148248</v>
+        <v>143.826887066846</v>
       </c>
       <c r="S21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="3" t="n">
+        <f aca="false">-I21</f>
+        <v>143.8</v>
+      </c>
+      <c r="V21" s="3" t="n">
+        <f aca="false">R21</f>
+        <v>143.826887066846</v>
+      </c>
+      <c r="W21" s="3" t="n">
+        <f aca="false">-K21</f>
+        <v>0.002974</v>
+      </c>
+      <c r="X21" s="3" t="n">
+        <f aca="false">S21</f>
         <v>0</v>
       </c>
     </row>
@@ -1189,34 +4547,34 @@
         <v>30</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>476.4</v>
+        <v>611.3</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>30</v>
+        <v>13.28</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>-0.1903</v>
+        <v>-1.484E-005</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>30</v>
+        <v>9.528</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>-143.1</v>
+        <v>-131.6</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K22" s="0" t="n">
-        <v>-333.2</v>
+        <v>2.707E-008</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>-479.7</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>476.4</v>
+        <v>611.3</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>-143.1</v>
+        <v>-131.6</v>
       </c>
       <c r="N22" s="2" t="n">
-        <v>-333.2</v>
+        <v>-479.7</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="0" t="n">
@@ -1226,10 +4584,27 @@
         <v>30</v>
       </c>
       <c r="R22" s="2" t="n">
-        <v>143.088857845281</v>
+        <v>131.559944121506</v>
       </c>
       <c r="S22" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>500</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="3" t="n">
+        <f aca="false">-I22</f>
+        <v>131.6</v>
+      </c>
+      <c r="V22" s="3" t="n">
+        <f aca="false">R22</f>
+        <v>131.559944121506</v>
+      </c>
+      <c r="W22" s="3" t="n">
+        <f aca="false">-K22</f>
+        <v>479.7</v>
+      </c>
+      <c r="X22" s="3" t="n">
+        <f aca="false">S22</f>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="23">
@@ -1240,34 +4615,34 @@
         <v>30</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>467.3</v>
+        <v>603.1</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>30</v>
+        <v>13.69</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>-0.03483</v>
+        <v>7.45E-005</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>30</v>
+        <v>10.74</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>-134</v>
+        <v>-115.2</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <v>-333.3</v>
+        <v>2.343E-008</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>-487.9</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>467.3</v>
+        <v>603.1</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>-134</v>
+        <v>-115.2</v>
       </c>
       <c r="N23" s="2" t="n">
-        <v>-333.3</v>
+        <v>-487.9</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="0" t="n">
@@ -1277,10 +4652,27 @@
         <v>30</v>
       </c>
       <c r="R23" s="2" t="n">
-        <v>133.993741268985</v>
+        <v>115.188734284174</v>
       </c>
       <c r="S23" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>500</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="3" t="n">
+        <f aca="false">-I23</f>
+        <v>115.2</v>
+      </c>
+      <c r="V23" s="3" t="n">
+        <f aca="false">R23</f>
+        <v>115.188734284174</v>
+      </c>
+      <c r="W23" s="3" t="n">
+        <f aca="false">-K23</f>
+        <v>487.9</v>
+      </c>
+      <c r="X23" s="3" t="n">
+        <f aca="false">S23</f>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="24">
@@ -1291,34 +4683,34 @@
         <v>30</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>458</v>
+        <v>594.7</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>30</v>
+        <v>14.11</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>-0.07771</v>
+        <v>-2.225E-005</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>30</v>
+        <v>11.86</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>-124.9</v>
+        <v>-98.8</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <v>-333.1</v>
+        <v>4.947E-009</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>-495.9</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>458</v>
+        <v>594.7</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>-124.9</v>
+        <v>-98.8</v>
       </c>
       <c r="N24" s="2" t="n">
-        <v>-333.1</v>
+        <v>-495.9</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="0" t="n">
@@ -1328,10 +4720,27 @@
         <v>30</v>
       </c>
       <c r="R24" s="2" t="n">
-        <v>124.864656003329</v>
+        <v>98.7563808059921</v>
       </c>
       <c r="S24" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>500</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="3" t="n">
+        <f aca="false">-I24</f>
+        <v>98.8</v>
+      </c>
+      <c r="V24" s="3" t="n">
+        <f aca="false">R24</f>
+        <v>98.7563808059921</v>
+      </c>
+      <c r="W24" s="3" t="n">
+        <f aca="false">-K24</f>
+        <v>495.9</v>
+      </c>
+      <c r="X24" s="3" t="n">
+        <f aca="false">S24</f>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="25">
@@ -1342,34 +4751,34 @@
         <v>30</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>452.1</v>
+        <v>587.9</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>30</v>
+        <v>14.44</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>-0.03894</v>
+        <v>-3.228E-005</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>30</v>
+        <v>12.62</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>-118.8</v>
+        <v>-87.9</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <v>-333.3</v>
+        <v>0.121</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>-500</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>452.1</v>
+        <v>587.9</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>-118.8</v>
+        <v>-87.9</v>
       </c>
       <c r="N25" s="2" t="n">
-        <v>-333.3</v>
+        <v>-500</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="0" t="n">
@@ -1379,10 +4788,27 @@
         <v>30</v>
       </c>
       <c r="R25" s="2" t="n">
-        <v>118.818229297145</v>
+        <v>87.8728127348616</v>
       </c>
       <c r="S25" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>500</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="3" t="n">
+        <f aca="false">-I25</f>
+        <v>87.9</v>
+      </c>
+      <c r="V25" s="3" t="n">
+        <f aca="false">R25</f>
+        <v>87.8728127348616</v>
+      </c>
+      <c r="W25" s="3" t="n">
+        <f aca="false">-K25</f>
+        <v>500</v>
+      </c>
+      <c r="X25" s="3" t="n">
+        <f aca="false">S25</f>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="26">
@@ -1393,34 +4819,34 @@
         <v>25</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>444.3</v>
+        <v>529.6</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>25</v>
+        <v>12.1</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>0.03087</v>
+        <v>0.0002828</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>25</v>
+        <v>10.76</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>-111</v>
+        <v>-73.7</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K26" s="0" t="n">
-        <v>-333.3</v>
+        <v>2.674E-007</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>-455.9</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>444.3</v>
+        <v>529.6</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>-111</v>
+        <v>-73.7</v>
       </c>
       <c r="N26" s="2" t="n">
-        <v>-333.3</v>
+        <v>-455.9</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="0" t="n">
@@ -1430,10 +4856,27 @@
         <v>25</v>
       </c>
       <c r="R26" s="2" t="n">
-        <v>110.954477710171</v>
+        <v>73.7180598783072</v>
       </c>
       <c r="S26" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>500</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="3" t="n">
+        <f aca="false">-I26</f>
+        <v>73.7</v>
+      </c>
+      <c r="V26" s="3" t="n">
+        <f aca="false">R26</f>
+        <v>73.7180598783072</v>
+      </c>
+      <c r="W26" s="3" t="n">
+        <f aca="false">-K26</f>
+        <v>455.9</v>
+      </c>
+      <c r="X26" s="3" t="n">
+        <f aca="false">S26</f>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="27">
@@ -1444,34 +4887,34 @@
         <v>25</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>432.2</v>
+        <v>518.3</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>25</v>
+        <v>12.6</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>0.101</v>
+        <v>5.153E-005</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>25</v>
+        <v>11.87</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>-98.99</v>
+        <v>-52.3</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K27" s="0" t="n">
-        <v>-333.3</v>
+        <v>1.148E-008</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>-466</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>432.2</v>
+        <v>518.3</v>
       </c>
       <c r="M27" s="0" t="n">
-        <v>-98.99</v>
+        <v>-52.3</v>
       </c>
       <c r="N27" s="2" t="n">
-        <v>-333.3</v>
+        <v>-466</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="0" t="n">
@@ -1481,10 +4924,27 @@
         <v>25</v>
       </c>
       <c r="R27" s="2" t="n">
-        <v>99.0442060031166</v>
+        <v>52.2795708056099</v>
       </c>
       <c r="S27" s="2" t="n">
-        <v>333.333333333333</v>
+        <v>500</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="3" t="n">
+        <f aca="false">-I27</f>
+        <v>52.3</v>
+      </c>
+      <c r="V27" s="3" t="n">
+        <f aca="false">R27</f>
+        <v>52.2795708056099</v>
+      </c>
+      <c r="W27" s="3" t="n">
+        <f aca="false">-K27</f>
+        <v>466</v>
+      </c>
+      <c r="X27" s="3" t="n">
+        <f aca="false">S27</f>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1495,6 +4955,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>